<commit_message>
Adds test for veg reset value function with tests around 25% of the conditions
</commit_message>
<xml_diff>
--- a/cord/data/ripcas_inputs/veg_roughness_shearres.xlsx
+++ b/cord/data/ripcas_inputs/veg_roughness_shearres.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Projects\CoRD\cord\data\ripcas_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254DE106-0F51-4413-9007-B3ED30509324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A114F098-1AE8-4334-A0F1-29AAC25B0FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1134,7 +1134,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1154,10 +1154,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1481,9 +1482,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL602"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AB1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AK2" sqref="AK2"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AA1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AF2" sqref="AF2:AK25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1630,25 +1631,25 @@
         <f>CONCATENATE(Y2,":",Z2,",")</f>
         <v>100:0.016,</v>
       </c>
-      <c r="AF2" s="13">
+      <c r="AF2" s="14">
         <v>1</v>
       </c>
-      <c r="AG2" s="13">
+      <c r="AG2" s="14">
         <v>100</v>
       </c>
-      <c r="AH2" s="13">
+      <c r="AH2" s="14">
         <v>100</v>
       </c>
-      <c r="AI2" s="13">
+      <c r="AI2" s="14">
         <v>1000</v>
       </c>
-      <c r="AJ2" s="13">
+      <c r="AJ2" s="14">
         <v>3999</v>
       </c>
-      <c r="AK2" s="13">
+      <c r="AK2" s="14">
         <v>1000</v>
       </c>
-      <c r="AL2" s="14" t="s">
+      <c r="AL2" s="13" t="s">
         <v>301</v>
       </c>
     </row>
@@ -1710,22 +1711,22 @@
         <f t="shared" ref="AA3:AA66" si="3">CONCATENATE(Y3,":",Z3,",")</f>
         <v>101:0.016,</v>
       </c>
-      <c r="AF3">
+      <c r="AF3" s="15">
         <v>2</v>
       </c>
-      <c r="AG3">
+      <c r="AG3" s="15">
         <v>100</v>
       </c>
-      <c r="AH3">
+      <c r="AH3" s="15">
         <v>200</v>
       </c>
-      <c r="AI3">
+      <c r="AI3" s="15">
         <v>1000</v>
       </c>
-      <c r="AJ3">
+      <c r="AJ3" s="15">
         <v>3999</v>
       </c>
-      <c r="AK3">
+      <c r="AK3" s="15">
         <v>1000</v>
       </c>
       <c r="AL3" s="6" t="s">
@@ -1790,25 +1791,25 @@
         <f t="shared" si="3"/>
         <v>102:0.05,</v>
       </c>
-      <c r="AF4" s="13">
+      <c r="AF4" s="14">
         <v>3</v>
       </c>
-      <c r="AG4" s="13">
+      <c r="AG4" s="14">
         <v>100</v>
       </c>
-      <c r="AH4" s="13">
+      <c r="AH4" s="14">
         <v>300</v>
       </c>
-      <c r="AI4" s="13">
+      <c r="AI4" s="14">
         <v>1000</v>
       </c>
-      <c r="AJ4" s="13">
+      <c r="AJ4" s="14">
         <v>3999</v>
       </c>
-      <c r="AK4" s="13">
+      <c r="AK4" s="14">
         <v>1000</v>
       </c>
-      <c r="AL4" s="14" t="s">
+      <c r="AL4" s="13" t="s">
         <v>303</v>
       </c>
     </row>
@@ -1870,22 +1871,22 @@
         <f t="shared" si="3"/>
         <v>103:0.05,</v>
       </c>
-      <c r="AF5">
+      <c r="AF5" s="15">
         <v>4</v>
       </c>
-      <c r="AG5">
+      <c r="AG5" s="15">
         <v>200</v>
       </c>
-      <c r="AH5">
+      <c r="AH5" s="15">
         <v>100</v>
       </c>
-      <c r="AI5">
+      <c r="AI5" s="15">
         <v>1000</v>
       </c>
-      <c r="AJ5">
+      <c r="AJ5" s="15">
         <v>1999</v>
       </c>
-      <c r="AK5">
+      <c r="AK5" s="15">
         <v>1000</v>
       </c>
       <c r="AL5" s="6" t="s">
@@ -1950,25 +1951,25 @@
         <f t="shared" si="3"/>
         <v>104:0.2,</v>
       </c>
-      <c r="AF6" s="13">
+      <c r="AF6" s="14">
         <v>5</v>
       </c>
-      <c r="AG6" s="13">
+      <c r="AG6" s="14">
         <v>200</v>
       </c>
-      <c r="AH6" s="13">
+      <c r="AH6" s="14">
         <v>100</v>
       </c>
-      <c r="AI6" s="13">
+      <c r="AI6" s="14">
         <v>3000</v>
       </c>
-      <c r="AJ6" s="13">
+      <c r="AJ6" s="14">
         <v>3999</v>
       </c>
-      <c r="AK6" s="13">
+      <c r="AK6" s="14">
         <v>1000</v>
       </c>
-      <c r="AL6" s="14" t="s">
+      <c r="AL6" s="13" t="s">
         <v>305</v>
       </c>
     </row>
@@ -2030,22 +2031,22 @@
         <f t="shared" si="3"/>
         <v>105:0.2,</v>
       </c>
-      <c r="AF7">
+      <c r="AF7" s="15">
         <v>6</v>
       </c>
-      <c r="AG7">
+      <c r="AG7" s="15">
         <v>200</v>
       </c>
-      <c r="AH7">
+      <c r="AH7" s="15">
         <v>100</v>
       </c>
-      <c r="AI7">
+      <c r="AI7" s="15">
         <v>2000</v>
       </c>
-      <c r="AJ7">
+      <c r="AJ7" s="15">
         <v>2999</v>
       </c>
-      <c r="AK7">
+      <c r="AK7" s="15">
         <v>2000</v>
       </c>
       <c r="AL7" s="6" t="s">
@@ -2110,25 +2111,25 @@
         <f t="shared" si="3"/>
         <v>106:0.2,</v>
       </c>
-      <c r="AF8" s="13">
+      <c r="AF8" s="14">
         <v>7</v>
       </c>
-      <c r="AG8" s="13">
+      <c r="AG8" s="14">
         <v>200</v>
       </c>
-      <c r="AH8" s="13">
+      <c r="AH8" s="14">
         <v>200</v>
       </c>
-      <c r="AI8" s="13">
+      <c r="AI8" s="14">
         <v>1000</v>
       </c>
-      <c r="AJ8" s="13">
+      <c r="AJ8" s="14">
         <v>1999</v>
       </c>
-      <c r="AK8" s="13">
+      <c r="AK8" s="14">
         <v>1000</v>
       </c>
-      <c r="AL8" s="14" t="s">
+      <c r="AL8" s="13" t="s">
         <v>307</v>
       </c>
     </row>
@@ -2190,22 +2191,22 @@
         <f t="shared" si="3"/>
         <v>107:0.2,</v>
       </c>
-      <c r="AF9">
+      <c r="AF9" s="15">
         <v>8</v>
       </c>
-      <c r="AG9">
+      <c r="AG9" s="15">
         <v>200</v>
       </c>
-      <c r="AH9">
+      <c r="AH9" s="15">
         <v>200</v>
       </c>
-      <c r="AI9">
+      <c r="AI9" s="15">
         <v>3000</v>
       </c>
-      <c r="AJ9">
+      <c r="AJ9" s="15">
         <v>3999</v>
       </c>
-      <c r="AK9">
+      <c r="AK9" s="15">
         <v>1000</v>
       </c>
       <c r="AL9" s="6" t="s">
@@ -2270,25 +2271,25 @@
         <f t="shared" si="3"/>
         <v>108:0.2,</v>
       </c>
-      <c r="AF10" s="13">
+      <c r="AF10" s="14">
         <v>9</v>
       </c>
-      <c r="AG10" s="13">
+      <c r="AG10" s="14">
         <v>200</v>
       </c>
-      <c r="AH10" s="13">
+      <c r="AH10" s="14">
         <v>200</v>
       </c>
-      <c r="AI10" s="13">
+      <c r="AI10" s="14">
         <v>2000</v>
       </c>
-      <c r="AJ10" s="13">
+      <c r="AJ10" s="14">
         <v>2999</v>
       </c>
-      <c r="AK10" s="13">
+      <c r="AK10" s="14">
         <v>2000</v>
       </c>
-      <c r="AL10" s="14" t="s">
+      <c r="AL10" s="13" t="s">
         <v>309</v>
       </c>
     </row>
@@ -2350,22 +2351,22 @@
         <f t="shared" si="3"/>
         <v>109:0.2,</v>
       </c>
-      <c r="AF11">
+      <c r="AF11" s="15">
         <v>10</v>
       </c>
-      <c r="AG11">
+      <c r="AG11" s="15">
         <v>200</v>
       </c>
-      <c r="AH11">
+      <c r="AH11" s="15">
         <v>300</v>
       </c>
-      <c r="AI11">
+      <c r="AI11" s="15">
         <v>1000</v>
       </c>
-      <c r="AJ11">
+      <c r="AJ11" s="15">
         <v>1999</v>
       </c>
-      <c r="AK11">
+      <c r="AK11" s="15">
         <v>1000</v>
       </c>
       <c r="AL11" s="6" t="s">
@@ -2430,25 +2431,25 @@
         <f t="shared" si="3"/>
         <v>110:0.2,</v>
       </c>
-      <c r="AF12" s="13">
+      <c r="AF12" s="14">
         <v>11</v>
       </c>
-      <c r="AG12" s="13">
+      <c r="AG12" s="14">
         <v>200</v>
       </c>
-      <c r="AH12" s="13">
+      <c r="AH12" s="14">
         <v>300</v>
       </c>
-      <c r="AI12" s="13">
+      <c r="AI12" s="14">
         <v>3000</v>
       </c>
-      <c r="AJ12" s="13">
+      <c r="AJ12" s="14">
         <v>3999</v>
       </c>
-      <c r="AK12" s="13">
+      <c r="AK12" s="14">
         <v>3000</v>
       </c>
-      <c r="AL12" s="14" t="s">
+      <c r="AL12" s="13" t="s">
         <v>311</v>
       </c>
     </row>
@@ -2510,22 +2511,22 @@
         <f t="shared" si="3"/>
         <v>111:0.15,</v>
       </c>
-      <c r="AF13">
+      <c r="AF13" s="15">
         <v>12</v>
       </c>
-      <c r="AG13">
+      <c r="AG13" s="15">
         <v>200</v>
       </c>
-      <c r="AH13">
+      <c r="AH13" s="15">
         <v>300</v>
       </c>
-      <c r="AI13">
+      <c r="AI13" s="15">
         <v>2000</v>
       </c>
-      <c r="AJ13">
+      <c r="AJ13" s="15">
         <v>2999</v>
       </c>
-      <c r="AK13">
+      <c r="AK13" s="15">
         <v>2000</v>
       </c>
       <c r="AL13" s="6" t="s">
@@ -2575,25 +2576,25 @@
         <f t="shared" si="3"/>
         <v>112:0.15,</v>
       </c>
-      <c r="AF14" s="13">
+      <c r="AF14" s="14">
         <v>13</v>
       </c>
-      <c r="AG14" s="13">
+      <c r="AG14" s="14">
         <v>300</v>
       </c>
-      <c r="AH14" s="13">
+      <c r="AH14" s="14">
         <v>100</v>
       </c>
-      <c r="AI14" s="13">
+      <c r="AI14" s="14">
         <v>1000</v>
       </c>
-      <c r="AJ14" s="13">
+      <c r="AJ14" s="14">
         <v>1999</v>
       </c>
-      <c r="AK14" s="13">
+      <c r="AK14" s="14">
         <v>1000</v>
       </c>
-      <c r="AL14" s="14" t="s">
+      <c r="AL14" s="13" t="s">
         <v>313</v>
       </c>
     </row>
@@ -2658,22 +2659,22 @@
         <f t="shared" si="3"/>
         <v>113:0.15,</v>
       </c>
-      <c r="AF15">
+      <c r="AF15" s="15">
         <v>14</v>
       </c>
-      <c r="AG15">
+      <c r="AG15" s="15">
         <v>300</v>
       </c>
-      <c r="AH15">
+      <c r="AH15" s="15">
         <v>100</v>
       </c>
-      <c r="AI15">
+      <c r="AI15" s="15">
         <v>2000</v>
       </c>
-      <c r="AJ15">
+      <c r="AJ15" s="15">
         <v>2999</v>
       </c>
-      <c r="AK15">
+      <c r="AK15" s="15">
         <v>2000</v>
       </c>
       <c r="AL15" s="6" t="s">
@@ -2754,25 +2755,25 @@
         <f t="shared" si="3"/>
         <v>114:0.15,</v>
       </c>
-      <c r="AF16" s="13">
+      <c r="AF16" s="14">
         <v>15</v>
       </c>
-      <c r="AG16" s="13">
+      <c r="AG16" s="14">
         <v>300</v>
       </c>
-      <c r="AH16" s="13">
+      <c r="AH16" s="14">
         <v>100</v>
       </c>
-      <c r="AI16" s="13">
+      <c r="AI16" s="14">
         <v>3000</v>
       </c>
-      <c r="AJ16" s="13">
+      <c r="AJ16" s="14">
         <v>3999</v>
       </c>
-      <c r="AK16" s="13">
+      <c r="AK16" s="14">
         <v>3000</v>
       </c>
-      <c r="AL16" s="14" t="s">
+      <c r="AL16" s="13" t="s">
         <v>315</v>
       </c>
     </row>
@@ -2841,22 +2842,22 @@
         <f t="shared" si="3"/>
         <v>115:0.15,</v>
       </c>
-      <c r="AF17">
+      <c r="AF17" s="15">
         <v>16</v>
       </c>
-      <c r="AG17">
+      <c r="AG17" s="15">
         <v>300</v>
       </c>
-      <c r="AH17">
+      <c r="AH17" s="15">
         <v>200</v>
       </c>
-      <c r="AI17">
+      <c r="AI17" s="15">
         <v>1000</v>
       </c>
-      <c r="AJ17">
+      <c r="AJ17" s="15">
         <v>1999</v>
       </c>
-      <c r="AK17">
+      <c r="AK17" s="15">
         <v>1000</v>
       </c>
       <c r="AL17" s="6" t="s">
@@ -2928,25 +2929,25 @@
         <f t="shared" si="3"/>
         <v>116:0.15,</v>
       </c>
-      <c r="AF18" s="13">
+      <c r="AF18" s="14">
         <v>17</v>
       </c>
-      <c r="AG18" s="13">
+      <c r="AG18" s="14">
         <v>300</v>
       </c>
-      <c r="AH18" s="13">
+      <c r="AH18" s="14">
         <v>200</v>
       </c>
-      <c r="AI18" s="13">
+      <c r="AI18" s="14">
         <v>2000</v>
       </c>
-      <c r="AJ18" s="13">
+      <c r="AJ18" s="14">
         <v>2999</v>
       </c>
-      <c r="AK18" s="13">
+      <c r="AK18" s="14">
         <v>2000</v>
       </c>
-      <c r="AL18" s="14" t="s">
+      <c r="AL18" s="13" t="s">
         <v>317</v>
       </c>
     </row>
@@ -3015,22 +3016,22 @@
         <f t="shared" si="3"/>
         <v>117:0.15,</v>
       </c>
-      <c r="AF19">
+      <c r="AF19" s="15">
         <v>18</v>
       </c>
-      <c r="AG19">
+      <c r="AG19" s="15">
         <v>300</v>
       </c>
-      <c r="AH19">
+      <c r="AH19" s="15">
         <v>200</v>
       </c>
-      <c r="AI19">
+      <c r="AI19" s="15">
         <v>3000</v>
       </c>
-      <c r="AJ19">
+      <c r="AJ19" s="15">
         <v>3999</v>
       </c>
-      <c r="AK19">
+      <c r="AK19" s="15">
         <v>3000</v>
       </c>
       <c r="AL19" s="6" t="s">
@@ -3102,25 +3103,25 @@
         <f t="shared" si="3"/>
         <v>118:0.15,</v>
       </c>
-      <c r="AF20" s="13">
+      <c r="AF20" s="14">
         <v>19</v>
       </c>
-      <c r="AG20" s="13">
+      <c r="AG20" s="14">
         <v>300</v>
       </c>
-      <c r="AH20" s="13">
+      <c r="AH20" s="14">
         <v>300</v>
       </c>
-      <c r="AI20" s="13">
+      <c r="AI20" s="14">
         <v>1000</v>
       </c>
-      <c r="AJ20" s="13">
+      <c r="AJ20" s="14">
         <v>1999</v>
       </c>
-      <c r="AK20" s="13">
+      <c r="AK20" s="14">
         <v>3000</v>
       </c>
-      <c r="AL20" s="14" t="s">
+      <c r="AL20" s="13" t="s">
         <v>319</v>
       </c>
     </row>
@@ -3189,22 +3190,22 @@
         <f t="shared" si="3"/>
         <v>119:0.15,</v>
       </c>
-      <c r="AF21">
+      <c r="AF21" s="15">
         <v>20</v>
       </c>
-      <c r="AG21">
+      <c r="AG21" s="15">
         <v>300</v>
       </c>
-      <c r="AH21">
+      <c r="AH21" s="15">
         <v>300</v>
       </c>
-      <c r="AI21">
+      <c r="AI21" s="15">
         <v>2000</v>
       </c>
-      <c r="AJ21">
+      <c r="AJ21" s="15">
         <v>2999</v>
       </c>
-      <c r="AK21">
+      <c r="AK21" s="15">
         <v>2000</v>
       </c>
       <c r="AL21" s="6" t="s">
@@ -3285,25 +3286,25 @@
         <f t="shared" si="3"/>
         <v>120:0.15,</v>
       </c>
-      <c r="AF22" s="13">
+      <c r="AF22" s="14">
         <v>21</v>
       </c>
-      <c r="AG22" s="13">
+      <c r="AG22" s="14">
         <v>300</v>
       </c>
-      <c r="AH22" s="13">
+      <c r="AH22" s="14">
         <v>300</v>
       </c>
-      <c r="AI22" s="13">
+      <c r="AI22" s="14">
         <v>3000</v>
       </c>
-      <c r="AJ22" s="13">
+      <c r="AJ22" s="14">
         <v>3999</v>
       </c>
-      <c r="AK22" s="13">
+      <c r="AK22" s="14">
         <v>2000</v>
       </c>
-      <c r="AL22" s="14" t="s">
+      <c r="AL22" s="13" t="s">
         <v>321</v>
       </c>
     </row>
@@ -3372,22 +3373,22 @@
         <f t="shared" si="3"/>
         <v>121:0.15,</v>
       </c>
-      <c r="AF23">
+      <c r="AF23" s="15">
         <v>22</v>
       </c>
-      <c r="AG23">
+      <c r="AG23" s="15">
         <v>400</v>
       </c>
-      <c r="AH23">
+      <c r="AH23" s="15">
         <v>100</v>
       </c>
-      <c r="AI23">
+      <c r="AI23" s="15">
         <v>1000</v>
       </c>
-      <c r="AJ23">
+      <c r="AJ23" s="15">
         <v>3999</v>
       </c>
-      <c r="AK23">
+      <c r="AK23" s="15">
         <v>2000</v>
       </c>
       <c r="AL23" s="6" t="s">
@@ -3459,25 +3460,25 @@
         <f t="shared" si="3"/>
         <v>122:0.15,</v>
       </c>
-      <c r="AF24" s="13">
+      <c r="AF24" s="14">
         <v>23</v>
       </c>
-      <c r="AG24" s="13">
+      <c r="AG24" s="14">
         <v>400</v>
       </c>
-      <c r="AH24" s="13">
+      <c r="AH24" s="14">
         <v>200</v>
       </c>
-      <c r="AI24" s="13">
+      <c r="AI24" s="14">
         <v>1000</v>
       </c>
-      <c r="AJ24" s="13">
+      <c r="AJ24" s="14">
         <v>3999</v>
       </c>
-      <c r="AK24" s="13">
+      <c r="AK24" s="14">
         <v>2000</v>
       </c>
-      <c r="AL24" s="14" t="s">
+      <c r="AL24" s="13" t="s">
         <v>323</v>
       </c>
     </row>
@@ -3546,22 +3547,22 @@
         <f t="shared" si="3"/>
         <v>123:0.15,</v>
       </c>
-      <c r="AF25">
+      <c r="AF25" s="15">
         <v>24</v>
       </c>
-      <c r="AG25">
+      <c r="AG25" s="15">
         <v>400</v>
       </c>
-      <c r="AH25">
+      <c r="AH25" s="15">
         <v>300</v>
       </c>
-      <c r="AI25">
+      <c r="AI25" s="15">
         <v>1000</v>
       </c>
-      <c r="AJ25">
+      <c r="AJ25" s="15">
         <v>3999</v>
       </c>
-      <c r="AK25">
+      <c r="AK25" s="15">
         <v>2000</v>
       </c>
       <c r="AL25" s="6" t="s">
@@ -22363,7 +22364,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>